<commit_message>
feat(condo): DOMA-8525 ability to set Meter.isAutomatic via meters import
</commit_message>
<xml_diff>
--- a/apps/condo/public/import/meter/en/meter-import-example.xlsx
+++ b/apps/condo/public/import/meter/en/meter-import-example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>Address</t>
   </si>
@@ -70,12 +70,21 @@
     <t>Meter place</t>
   </si>
   <si>
+    <t>Automatic</t>
+  </si>
+  <si>
     <t>г Москва, ул Тверская, д 1</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>Flat</t>
   </si>
   <si>
+    <t>111</t>
+  </si>
+  <si>
     <t>HW</t>
   </si>
   <si>
@@ -112,12 +121,12 @@
     <t>CW</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>Warehouse unit</t>
   </si>
   <si>
-    <t>2021-12</t>
-  </si>
-  <si>
     <t>Commercial unit</t>
   </si>
   <si>
@@ -130,23 +139,33 @@
     <t>г Москва, ул Тверская, д 2</t>
   </si>
   <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>2021-12-21</t>
   </si>
   <si>
     <t>HEAT</t>
   </si>
   <si>
+    <t>22</t>
+  </si>
+  <si>
     <t>GAS</t>
+  </si>
+  <si>
+    <t>33</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="d&quot;.&quot;mm&quot;.&quot;yyyy"/>
-    <numFmt numFmtId="60" formatCode="dd&quot;.&quot;mm&quot;.&quot;yyyy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -271,7 +290,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -303,15 +322,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1369,7 +1379,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1389,8 +1399,8 @@
     <col min="15" max="15" width="12.8516" style="1" customWidth="1"/>
     <col min="16" max="16" width="22.1719" style="1" customWidth="1"/>
     <col min="17" max="17" width="18.1719" style="1" customWidth="1"/>
-    <col min="18" max="19" width="23.5" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="18" max="20" width="23.5" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.75" customHeight="1">
@@ -1451,25 +1461,28 @@
       <c r="S1" t="s" s="7">
         <v>18</v>
       </c>
+      <c r="T1" t="s" s="7">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" ht="13.75" customHeight="1">
       <c r="A2" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="B2" t="s" s="8">
+        <v>21</v>
       </c>
       <c r="C2" t="s" s="8">
-        <v>20</v>
-      </c>
-      <c r="D2" s="9">
-        <v>111</v>
+        <v>22</v>
+      </c>
+      <c r="D2" t="s" s="8">
+        <v>23</v>
       </c>
       <c r="E2" t="s" s="8">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s" s="8">
         <v>21</v>
-      </c>
-      <c r="F2" s="9">
-        <v>1</v>
       </c>
       <c r="G2" s="9">
         <v>1</v>
@@ -1477,52 +1490,53 @@
       <c r="H2" s="10">
         <v>100</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
       <c r="L2" t="s" s="7">
-        <v>22</v>
-      </c>
-      <c r="M2" s="12">
-        <v>44216</v>
+        <v>25</v>
+      </c>
+      <c r="M2" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N2" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O2" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P2" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q2" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R2" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S2" t="s" s="7">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="T2" s="7"/>
     </row>
     <row r="3" ht="13.75" customHeight="1">
       <c r="A3" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="B3" s="10">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="B3" t="s" s="7">
+        <v>21</v>
       </c>
       <c r="C3" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="D3" s="10">
-        <v>111</v>
+        <v>32</v>
+      </c>
+      <c r="D3" t="s" s="7">
+        <v>23</v>
       </c>
       <c r="E3" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s" s="7">
         <v>21</v>
-      </c>
-      <c r="F3" s="10">
-        <v>1</v>
       </c>
       <c r="G3" s="10">
         <v>1</v>
@@ -1530,52 +1544,53 @@
       <c r="H3" s="10">
         <v>200</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
       <c r="L3" t="s" s="7">
-        <v>22</v>
-      </c>
-      <c r="M3" s="12">
-        <v>44216</v>
+        <v>25</v>
+      </c>
+      <c r="M3" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N3" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O3" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P3" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q3" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R3" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S3" t="s" s="7">
-        <v>30</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="T3" s="7"/>
     </row>
     <row r="4" ht="13.75" customHeight="1">
       <c r="A4" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="B4" s="10">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="B4" t="s" s="7">
+        <v>21</v>
       </c>
       <c r="C4" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="D4" s="10">
-        <v>111</v>
+        <v>34</v>
+      </c>
+      <c r="D4" t="s" s="7">
+        <v>23</v>
       </c>
       <c r="E4" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="F4" s="10">
-        <v>2</v>
+        <v>35</v>
+      </c>
+      <c r="F4" t="s" s="7">
+        <v>36</v>
       </c>
       <c r="G4" s="10">
         <v>1</v>
@@ -1583,52 +1598,53 @@
       <c r="H4" s="10">
         <v>110</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
       <c r="L4" t="s" s="7">
-        <v>22</v>
-      </c>
-      <c r="M4" s="12">
-        <v>44216</v>
+        <v>25</v>
+      </c>
+      <c r="M4" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N4" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O4" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P4" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q4" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R4" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S4" t="s" s="7">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="T4" s="7"/>
     </row>
     <row r="5" ht="13.75" customHeight="1">
       <c r="A5" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="B5" s="10">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="B5" t="s" s="7">
+        <v>21</v>
       </c>
       <c r="C5" t="s" s="7">
-        <v>33</v>
-      </c>
-      <c r="D5" s="10">
-        <v>111</v>
+        <v>37</v>
+      </c>
+      <c r="D5" t="s" s="7">
+        <v>23</v>
       </c>
       <c r="E5" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="F5" s="10">
-        <v>2</v>
+        <v>35</v>
+      </c>
+      <c r="F5" t="s" s="7">
+        <v>36</v>
       </c>
       <c r="G5" s="10">
         <v>1</v>
@@ -1636,52 +1652,53 @@
       <c r="H5" s="10">
         <v>300</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
       <c r="L5" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="M5" s="12">
-        <v>44216</v>
+        <v>25</v>
+      </c>
+      <c r="M5" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N5" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O5" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P5" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q5" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R5" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S5" t="s" s="7">
-        <v>30</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="T5" s="7"/>
     </row>
     <row r="6" ht="13.75" customHeight="1">
       <c r="A6" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="B6" s="10">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="B6" t="s" s="7">
+        <v>21</v>
       </c>
       <c r="C6" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="D6" s="10">
-        <v>111</v>
+        <v>38</v>
+      </c>
+      <c r="D6" t="s" s="7">
+        <v>23</v>
       </c>
       <c r="E6" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s" s="7">
         <v>36</v>
-      </c>
-      <c r="F6" s="10">
-        <v>2</v>
       </c>
       <c r="G6" s="10">
         <v>3</v>
@@ -1695,50 +1712,51 @@
       <c r="J6" s="10">
         <v>508</v>
       </c>
-      <c r="K6" s="11"/>
+      <c r="K6" s="10"/>
       <c r="L6" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="M6" s="12">
-        <v>44216</v>
+        <v>40</v>
+      </c>
+      <c r="M6" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N6" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O6" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P6" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q6" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R6" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S6" t="s" s="7">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="T6" s="7"/>
     </row>
     <row r="7" ht="13.75" customHeight="1">
       <c r="A7" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="B7" s="10">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="B7" t="s" s="7">
+        <v>21</v>
       </c>
       <c r="C7" t="s" s="7">
-        <v>20</v>
-      </c>
-      <c r="D7" s="10">
-        <v>111</v>
+        <v>22</v>
+      </c>
+      <c r="D7" t="s" s="7">
+        <v>23</v>
       </c>
       <c r="E7" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s" s="7">
         <v>36</v>
-      </c>
-      <c r="F7" s="10">
-        <v>2</v>
       </c>
       <c r="G7" s="10">
         <v>3</v>
@@ -1752,50 +1770,51 @@
       <c r="J7" s="10">
         <v>584</v>
       </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="13">
-        <v>44550</v>
-      </c>
-      <c r="M7" s="12">
-        <v>44216</v>
+      <c r="K7" s="10"/>
+      <c r="L7" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="M7" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N7" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O7" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P7" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q7" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R7" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S7" t="s" s="7">
-        <v>30</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="T7" s="7"/>
     </row>
     <row r="8" ht="13.75" customHeight="1">
       <c r="A8" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="B8" s="10">
-        <v>2</v>
+        <v>41</v>
+      </c>
+      <c r="B8" t="s" s="7">
+        <v>36</v>
       </c>
       <c r="C8" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="D8" s="10">
-        <v>222</v>
+        <v>32</v>
+      </c>
+      <c r="D8" t="s" s="7">
+        <v>42</v>
       </c>
       <c r="E8" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="F8" s="10">
-        <v>11</v>
+        <v>39</v>
+      </c>
+      <c r="F8" t="s" s="7">
+        <v>43</v>
       </c>
       <c r="G8" s="10">
         <v>3</v>
@@ -1809,50 +1828,51 @@
       <c r="J8" s="10">
         <v>304</v>
       </c>
-      <c r="K8" s="11"/>
+      <c r="K8" s="10"/>
       <c r="L8" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="M8" s="12">
-        <v>44216</v>
+        <v>44</v>
+      </c>
+      <c r="M8" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N8" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O8" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P8" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q8" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R8" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S8" t="s" s="7">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="T8" s="7"/>
     </row>
     <row r="9" ht="13.75" customHeight="1">
       <c r="A9" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="B9" s="10">
-        <v>2</v>
+        <v>41</v>
+      </c>
+      <c r="B9" t="s" s="7">
+        <v>36</v>
       </c>
       <c r="C9" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="D9" s="10">
-        <v>222</v>
+        <v>32</v>
+      </c>
+      <c r="D9" t="s" s="7">
+        <v>42</v>
       </c>
       <c r="E9" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="F9" s="10">
-        <v>11</v>
+        <v>45</v>
+      </c>
+      <c r="F9" t="s" s="7">
+        <v>43</v>
       </c>
       <c r="G9" s="10">
         <v>1</v>
@@ -1860,52 +1880,53 @@
       <c r="H9" s="10">
         <v>238</v>
       </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
       <c r="L9" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="M9" s="12">
-        <v>44216</v>
+        <v>44</v>
+      </c>
+      <c r="M9" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N9" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O9" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P9" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q9" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R9" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S9" t="s" s="7">
-        <v>30</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="T9" s="7"/>
     </row>
     <row r="10" ht="13.75" customHeight="1">
       <c r="A10" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="B10" s="10">
-        <v>2</v>
+        <v>41</v>
+      </c>
+      <c r="B10" t="s" s="7">
+        <v>36</v>
       </c>
       <c r="C10" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="D10" s="10">
-        <v>222</v>
+        <v>32</v>
+      </c>
+      <c r="D10" t="s" s="7">
+        <v>42</v>
       </c>
       <c r="E10" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="F10" s="10">
-        <v>22</v>
+        <v>45</v>
+      </c>
+      <c r="F10" t="s" s="7">
+        <v>46</v>
       </c>
       <c r="G10" s="10">
         <v>1</v>
@@ -1913,52 +1934,53 @@
       <c r="H10" s="10">
         <v>294</v>
       </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
       <c r="L10" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="M10" s="12">
-        <v>44216</v>
+        <v>25</v>
+      </c>
+      <c r="M10" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N10" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O10" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P10" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q10" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R10" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S10" t="s" s="7">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="T10" s="7"/>
     </row>
     <row r="11" ht="13.75" customHeight="1">
       <c r="A11" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="B11" s="10">
-        <v>2</v>
+        <v>41</v>
+      </c>
+      <c r="B11" t="s" s="7">
+        <v>36</v>
       </c>
       <c r="C11" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="D11" s="10">
-        <v>222</v>
+        <v>32</v>
+      </c>
+      <c r="D11" t="s" s="7">
+        <v>42</v>
       </c>
       <c r="E11" t="s" s="7">
-        <v>41</v>
-      </c>
-      <c r="F11" s="10">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="F11" t="s" s="7">
+        <v>48</v>
       </c>
       <c r="G11" s="10">
         <v>1</v>
@@ -1966,33 +1988,34 @@
       <c r="H11" s="10">
         <v>338</v>
       </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
       <c r="L11" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="M11" s="12">
-        <v>44216</v>
+        <v>25</v>
+      </c>
+      <c r="M11" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N11" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O11" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P11" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q11" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R11" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S11" t="s" s="7">
-        <v>30</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="T11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
feat(condo): DOMA-8525 allow to restrict send meter readings (#4982)
* feat(condo): DOMA-8525 allow meter to be automatic without b2b-app

* feat(condo): DOMA-8525 ability to set Meter.isAutomatic via meters import

* feat(condo): DOMA-8525 fix tests for rows transformation

* feat(condo): DOMA-8525 Test was improved

Add testing of case when we need to keep existing value for isAutomatic if this value is not passed ti mutation

* feat(condo): DOMA-8525 Fix test with Excel files

* feat(condo): DOMA-8525 remove unused fields

* feat(condo): DOMA-8525 localized values for isAutomatic field

* feat(condo): DOMA-8525 improve tests

* feat(condo): DOMA-8525 comment improved

* feat(condo): DOMA-8525 logic improved a bit
</commit_message>
<xml_diff>
--- a/apps/condo/public/import/meter/en/meter-import-example.xlsx
+++ b/apps/condo/public/import/meter/en/meter-import-example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>Address</t>
   </si>
@@ -70,12 +70,21 @@
     <t>Meter place</t>
   </si>
   <si>
+    <t>Automatic</t>
+  </si>
+  <si>
     <t>г Москва, ул Тверская, д 1</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>Flat</t>
   </si>
   <si>
+    <t>111</t>
+  </si>
+  <si>
     <t>HW</t>
   </si>
   <si>
@@ -112,12 +121,12 @@
     <t>CW</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>Warehouse unit</t>
   </si>
   <si>
-    <t>2021-12</t>
-  </si>
-  <si>
     <t>Commercial unit</t>
   </si>
   <si>
@@ -130,23 +139,33 @@
     <t>г Москва, ул Тверская, д 2</t>
   </si>
   <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>2021-12-21</t>
   </si>
   <si>
     <t>HEAT</t>
   </si>
   <si>
+    <t>22</t>
+  </si>
+  <si>
     <t>GAS</t>
+  </si>
+  <si>
+    <t>33</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="d&quot;.&quot;mm&quot;.&quot;yyyy"/>
-    <numFmt numFmtId="60" formatCode="dd&quot;.&quot;mm&quot;.&quot;yyyy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -271,7 +290,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -303,15 +322,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1369,7 +1379,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1389,8 +1399,8 @@
     <col min="15" max="15" width="12.8516" style="1" customWidth="1"/>
     <col min="16" max="16" width="22.1719" style="1" customWidth="1"/>
     <col min="17" max="17" width="18.1719" style="1" customWidth="1"/>
-    <col min="18" max="19" width="23.5" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="18" max="20" width="23.5" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.75" customHeight="1">
@@ -1451,25 +1461,28 @@
       <c r="S1" t="s" s="7">
         <v>18</v>
       </c>
+      <c r="T1" t="s" s="7">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" ht="13.75" customHeight="1">
       <c r="A2" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="B2" t="s" s="8">
+        <v>21</v>
       </c>
       <c r="C2" t="s" s="8">
-        <v>20</v>
-      </c>
-      <c r="D2" s="9">
-        <v>111</v>
+        <v>22</v>
+      </c>
+      <c r="D2" t="s" s="8">
+        <v>23</v>
       </c>
       <c r="E2" t="s" s="8">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s" s="8">
         <v>21</v>
-      </c>
-      <c r="F2" s="9">
-        <v>1</v>
       </c>
       <c r="G2" s="9">
         <v>1</v>
@@ -1477,52 +1490,53 @@
       <c r="H2" s="10">
         <v>100</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
       <c r="L2" t="s" s="7">
-        <v>22</v>
-      </c>
-      <c r="M2" s="12">
-        <v>44216</v>
+        <v>25</v>
+      </c>
+      <c r="M2" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N2" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O2" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P2" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q2" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R2" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S2" t="s" s="7">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="T2" s="7"/>
     </row>
     <row r="3" ht="13.75" customHeight="1">
       <c r="A3" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="B3" s="10">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="B3" t="s" s="7">
+        <v>21</v>
       </c>
       <c r="C3" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="D3" s="10">
-        <v>111</v>
+        <v>32</v>
+      </c>
+      <c r="D3" t="s" s="7">
+        <v>23</v>
       </c>
       <c r="E3" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s" s="7">
         <v>21</v>
-      </c>
-      <c r="F3" s="10">
-        <v>1</v>
       </c>
       <c r="G3" s="10">
         <v>1</v>
@@ -1530,52 +1544,53 @@
       <c r="H3" s="10">
         <v>200</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
       <c r="L3" t="s" s="7">
-        <v>22</v>
-      </c>
-      <c r="M3" s="12">
-        <v>44216</v>
+        <v>25</v>
+      </c>
+      <c r="M3" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N3" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O3" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P3" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q3" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R3" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S3" t="s" s="7">
-        <v>30</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="T3" s="7"/>
     </row>
     <row r="4" ht="13.75" customHeight="1">
       <c r="A4" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="B4" s="10">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="B4" t="s" s="7">
+        <v>21</v>
       </c>
       <c r="C4" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="D4" s="10">
-        <v>111</v>
+        <v>34</v>
+      </c>
+      <c r="D4" t="s" s="7">
+        <v>23</v>
       </c>
       <c r="E4" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="F4" s="10">
-        <v>2</v>
+        <v>35</v>
+      </c>
+      <c r="F4" t="s" s="7">
+        <v>36</v>
       </c>
       <c r="G4" s="10">
         <v>1</v>
@@ -1583,52 +1598,53 @@
       <c r="H4" s="10">
         <v>110</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
       <c r="L4" t="s" s="7">
-        <v>22</v>
-      </c>
-      <c r="M4" s="12">
-        <v>44216</v>
+        <v>25</v>
+      </c>
+      <c r="M4" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N4" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O4" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P4" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q4" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R4" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S4" t="s" s="7">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="T4" s="7"/>
     </row>
     <row r="5" ht="13.75" customHeight="1">
       <c r="A5" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="B5" s="10">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="B5" t="s" s="7">
+        <v>21</v>
       </c>
       <c r="C5" t="s" s="7">
-        <v>33</v>
-      </c>
-      <c r="D5" s="10">
-        <v>111</v>
+        <v>37</v>
+      </c>
+      <c r="D5" t="s" s="7">
+        <v>23</v>
       </c>
       <c r="E5" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="F5" s="10">
-        <v>2</v>
+        <v>35</v>
+      </c>
+      <c r="F5" t="s" s="7">
+        <v>36</v>
       </c>
       <c r="G5" s="10">
         <v>1</v>
@@ -1636,52 +1652,53 @@
       <c r="H5" s="10">
         <v>300</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
       <c r="L5" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="M5" s="12">
-        <v>44216</v>
+        <v>25</v>
+      </c>
+      <c r="M5" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N5" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O5" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P5" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q5" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R5" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S5" t="s" s="7">
-        <v>30</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="T5" s="7"/>
     </row>
     <row r="6" ht="13.75" customHeight="1">
       <c r="A6" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="B6" s="10">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="B6" t="s" s="7">
+        <v>21</v>
       </c>
       <c r="C6" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="D6" s="10">
-        <v>111</v>
+        <v>38</v>
+      </c>
+      <c r="D6" t="s" s="7">
+        <v>23</v>
       </c>
       <c r="E6" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s" s="7">
         <v>36</v>
-      </c>
-      <c r="F6" s="10">
-        <v>2</v>
       </c>
       <c r="G6" s="10">
         <v>3</v>
@@ -1695,50 +1712,51 @@
       <c r="J6" s="10">
         <v>508</v>
       </c>
-      <c r="K6" s="11"/>
+      <c r="K6" s="10"/>
       <c r="L6" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="M6" s="12">
-        <v>44216</v>
+        <v>40</v>
+      </c>
+      <c r="M6" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N6" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O6" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P6" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q6" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R6" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S6" t="s" s="7">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="T6" s="7"/>
     </row>
     <row r="7" ht="13.75" customHeight="1">
       <c r="A7" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="B7" s="10">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="B7" t="s" s="7">
+        <v>21</v>
       </c>
       <c r="C7" t="s" s="7">
-        <v>20</v>
-      </c>
-      <c r="D7" s="10">
-        <v>111</v>
+        <v>22</v>
+      </c>
+      <c r="D7" t="s" s="7">
+        <v>23</v>
       </c>
       <c r="E7" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s" s="7">
         <v>36</v>
-      </c>
-      <c r="F7" s="10">
-        <v>2</v>
       </c>
       <c r="G7" s="10">
         <v>3</v>
@@ -1752,50 +1770,51 @@
       <c r="J7" s="10">
         <v>584</v>
       </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="13">
-        <v>44550</v>
-      </c>
-      <c r="M7" s="12">
-        <v>44216</v>
+      <c r="K7" s="10"/>
+      <c r="L7" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="M7" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N7" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O7" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P7" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q7" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R7" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S7" t="s" s="7">
-        <v>30</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="T7" s="7"/>
     </row>
     <row r="8" ht="13.75" customHeight="1">
       <c r="A8" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="B8" s="10">
-        <v>2</v>
+        <v>41</v>
+      </c>
+      <c r="B8" t="s" s="7">
+        <v>36</v>
       </c>
       <c r="C8" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="D8" s="10">
-        <v>222</v>
+        <v>32</v>
+      </c>
+      <c r="D8" t="s" s="7">
+        <v>42</v>
       </c>
       <c r="E8" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="F8" s="10">
-        <v>11</v>
+        <v>39</v>
+      </c>
+      <c r="F8" t="s" s="7">
+        <v>43</v>
       </c>
       <c r="G8" s="10">
         <v>3</v>
@@ -1809,50 +1828,51 @@
       <c r="J8" s="10">
         <v>304</v>
       </c>
-      <c r="K8" s="11"/>
+      <c r="K8" s="10"/>
       <c r="L8" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="M8" s="12">
-        <v>44216</v>
+        <v>44</v>
+      </c>
+      <c r="M8" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N8" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O8" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P8" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q8" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R8" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S8" t="s" s="7">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="T8" s="7"/>
     </row>
     <row r="9" ht="13.75" customHeight="1">
       <c r="A9" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="B9" s="10">
-        <v>2</v>
+        <v>41</v>
+      </c>
+      <c r="B9" t="s" s="7">
+        <v>36</v>
       </c>
       <c r="C9" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="D9" s="10">
-        <v>222</v>
+        <v>32</v>
+      </c>
+      <c r="D9" t="s" s="7">
+        <v>42</v>
       </c>
       <c r="E9" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="F9" s="10">
-        <v>11</v>
+        <v>45</v>
+      </c>
+      <c r="F9" t="s" s="7">
+        <v>43</v>
       </c>
       <c r="G9" s="10">
         <v>1</v>
@@ -1860,52 +1880,53 @@
       <c r="H9" s="10">
         <v>238</v>
       </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
       <c r="L9" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="M9" s="12">
-        <v>44216</v>
+        <v>44</v>
+      </c>
+      <c r="M9" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N9" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O9" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P9" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q9" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R9" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S9" t="s" s="7">
-        <v>30</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="T9" s="7"/>
     </row>
     <row r="10" ht="13.75" customHeight="1">
       <c r="A10" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="B10" s="10">
-        <v>2</v>
+        <v>41</v>
+      </c>
+      <c r="B10" t="s" s="7">
+        <v>36</v>
       </c>
       <c r="C10" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="D10" s="10">
-        <v>222</v>
+        <v>32</v>
+      </c>
+      <c r="D10" t="s" s="7">
+        <v>42</v>
       </c>
       <c r="E10" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="F10" s="10">
-        <v>22</v>
+        <v>45</v>
+      </c>
+      <c r="F10" t="s" s="7">
+        <v>46</v>
       </c>
       <c r="G10" s="10">
         <v>1</v>
@@ -1913,52 +1934,53 @@
       <c r="H10" s="10">
         <v>294</v>
       </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
       <c r="L10" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="M10" s="12">
-        <v>44216</v>
+        <v>25</v>
+      </c>
+      <c r="M10" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N10" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O10" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P10" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q10" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R10" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S10" t="s" s="7">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="T10" s="7"/>
     </row>
     <row r="11" ht="13.75" customHeight="1">
       <c r="A11" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="B11" s="10">
-        <v>2</v>
+        <v>41</v>
+      </c>
+      <c r="B11" t="s" s="7">
+        <v>36</v>
       </c>
       <c r="C11" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="D11" s="10">
-        <v>222</v>
+        <v>32</v>
+      </c>
+      <c r="D11" t="s" s="7">
+        <v>42</v>
       </c>
       <c r="E11" t="s" s="7">
-        <v>41</v>
-      </c>
-      <c r="F11" s="10">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="F11" t="s" s="7">
+        <v>48</v>
       </c>
       <c r="G11" s="10">
         <v>1</v>
@@ -1966,33 +1988,34 @@
       <c r="H11" s="10">
         <v>338</v>
       </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
       <c r="L11" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="M11" s="12">
-        <v>44216</v>
+        <v>25</v>
+      </c>
+      <c r="M11" t="s" s="7">
+        <v>25</v>
       </c>
       <c r="N11" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="O11" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P11" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q11" t="s" s="7">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R11" t="s" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S11" t="s" s="7">
-        <v>30</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="T11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
fix(condo): DOMA-11339 added archiveDate field in meters import
</commit_message>
<xml_diff>
--- a/apps/condo/public/import/meter/en/meter-import-example.xlsx
+++ b/apps/condo/public/import/meter/en/meter-import-example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>Address</t>
   </si>
@@ -73,6 +73,9 @@
     <t>Automatic</t>
   </si>
   <si>
+    <t>Archive date</t>
+  </si>
+  <si>
     <t>г Москва, ул Тверская, д 1</t>
   </si>
   <si>
@@ -107,6 +110,9 @@
   </si>
   <si>
     <t>Kitchen</t>
+  </si>
+  <si>
+    <t>2022-01-25</t>
   </si>
   <si>
     <t>Parking place</t>
@@ -290,7 +296,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -322,6 +328,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1379,7 +1388,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1399,8 +1408,8 @@
     <col min="15" max="15" width="12.8516" style="1" customWidth="1"/>
     <col min="16" max="16" width="22.1719" style="1" customWidth="1"/>
     <col min="17" max="17" width="18.1719" style="1" customWidth="1"/>
-    <col min="18" max="20" width="23.5" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="18" max="21" width="23.5" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.75" customHeight="1">
@@ -1464,25 +1473,28 @@
       <c r="T1" t="s" s="7">
         <v>19</v>
       </c>
+      <c r="U1" t="s" s="7">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" ht="13.75" customHeight="1">
       <c r="A2" t="s" s="8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s" s="8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s" s="8">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s" s="8">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s" s="8">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s" s="8">
         <v>22</v>
-      </c>
-      <c r="D2" t="s" s="8">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s" s="8">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s" s="8">
-        <v>21</v>
       </c>
       <c r="G2" s="9">
         <v>1</v>
@@ -1490,53 +1502,56 @@
       <c r="H2" s="10">
         <v>100</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
       <c r="L2" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M2" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N2" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O2" t="s" s="7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P2" t="s" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q2" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R2" t="s" s="7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S2" t="s" s="7">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T2" s="7"/>
+      <c r="U2" t="s" s="7">
+        <v>33</v>
+      </c>
     </row>
     <row r="3" ht="13.75" customHeight="1">
       <c r="A3" t="s" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s" s="7">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" s="10">
         <v>1</v>
@@ -1544,53 +1559,54 @@
       <c r="H3" s="10">
         <v>200</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
       <c r="L3" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M3" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N3" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O3" t="s" s="7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P3" t="s" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q3" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R3" t="s" s="7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S3" t="s" s="7">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
     </row>
     <row r="4" ht="13.75" customHeight="1">
       <c r="A4" t="s" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s" s="7">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s" s="7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s" s="7">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G4" s="10">
         <v>1</v>
@@ -1598,53 +1614,54 @@
       <c r="H4" s="10">
         <v>110</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
       <c r="L4" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M4" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N4" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O4" t="s" s="7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P4" t="s" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q4" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R4" t="s" s="7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S4" t="s" s="7">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
     </row>
     <row r="5" ht="13.75" customHeight="1">
       <c r="A5" t="s" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s" s="7">
         <v>37</v>
       </c>
-      <c r="D5" t="s" s="7">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s" s="7">
-        <v>35</v>
-      </c>
       <c r="F5" t="s" s="7">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G5" s="10">
         <v>1</v>
@@ -1652,53 +1669,54 @@
       <c r="H5" s="10">
         <v>300</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
       <c r="L5" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M5" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N5" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O5" t="s" s="7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P5" t="s" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q5" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R5" t="s" s="7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S5" t="s" s="7">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
     </row>
     <row r="6" ht="13.75" customHeight="1">
       <c r="A6" t="s" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s" s="7">
         <v>38</v>
-      </c>
-      <c r="D6" t="s" s="7">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="F6" t="s" s="7">
-        <v>36</v>
       </c>
       <c r="G6" s="10">
         <v>3</v>
@@ -1712,51 +1730,52 @@
       <c r="J6" s="10">
         <v>508</v>
       </c>
-      <c r="K6" s="10"/>
+      <c r="K6" s="11"/>
       <c r="L6" t="s" s="7">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="M6" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N6" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O6" t="s" s="7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P6" t="s" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q6" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R6" t="s" s="7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S6" t="s" s="7">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
     </row>
     <row r="7" ht="13.75" customHeight="1">
       <c r="A7" t="s" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s" s="7">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s" s="7">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G7" s="10">
         <v>3</v>
@@ -1770,51 +1789,52 @@
       <c r="J7" s="10">
         <v>584</v>
       </c>
-      <c r="K7" s="10"/>
+      <c r="K7" s="11"/>
       <c r="L7" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M7" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N7" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O7" t="s" s="7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P7" t="s" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q7" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R7" t="s" s="7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S7" t="s" s="7">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
     </row>
     <row r="8" ht="13.75" customHeight="1">
       <c r="A8" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s" s="7">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s" s="7">
         <v>41</v>
       </c>
-      <c r="B8" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="E8" t="s" s="7">
-        <v>39</v>
-      </c>
       <c r="F8" t="s" s="7">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G8" s="10">
         <v>3</v>
@@ -1828,51 +1848,52 @@
       <c r="J8" s="10">
         <v>304</v>
       </c>
-      <c r="K8" s="10"/>
+      <c r="K8" s="11"/>
       <c r="L8" t="s" s="7">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="M8" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N8" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O8" t="s" s="7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P8" t="s" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q8" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R8" t="s" s="7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S8" t="s" s="7">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
     </row>
     <row r="9" ht="13.75" customHeight="1">
       <c r="A9" t="s" s="7">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s" s="7">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s" s="7">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s" s="7">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s" s="7">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s" s="7">
         <v>45</v>
-      </c>
-      <c r="F9" t="s" s="7">
-        <v>43</v>
       </c>
       <c r="G9" s="10">
         <v>1</v>
@@ -1880,53 +1901,54 @@
       <c r="H9" s="10">
         <v>238</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
       <c r="L9" t="s" s="7">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="M9" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N9" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O9" t="s" s="7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P9" t="s" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q9" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R9" t="s" s="7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S9" t="s" s="7">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
     </row>
     <row r="10" ht="13.75" customHeight="1">
       <c r="A10" t="s" s="7">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s" s="7">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s" s="7">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s" s="7">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s" s="7">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s" s="7">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G10" s="10">
         <v>1</v>
@@ -1934,53 +1956,54 @@
       <c r="H10" s="10">
         <v>294</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
       <c r="L10" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M10" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N10" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O10" t="s" s="7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P10" t="s" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q10" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R10" t="s" s="7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S10" t="s" s="7">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
     </row>
     <row r="11" ht="13.75" customHeight="1">
       <c r="A11" t="s" s="7">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s" s="7">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s" s="7">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s" s="7">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s" s="7">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s" s="7">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G11" s="10">
         <v>1</v>
@@ -1988,34 +2011,35 @@
       <c r="H11" s="10">
         <v>338</v>
       </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
       <c r="L11" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M11" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N11" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O11" t="s" s="7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P11" t="s" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q11" t="s" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R11" t="s" s="7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S11" t="s" s="7">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>